<commit_message>
Added reproducibility for neural networks
</commit_message>
<xml_diff>
--- a/predictions/classical_predictions.xlsx
+++ b/predictions/classical_predictions.xlsx
@@ -467,10 +467,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5603867769241333</v>
+        <v>0.4480947554111481</v>
       </c>
     </row>
     <row r="3">
@@ -488,7 +488,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3992350995540619</v>
+        <v>0.3647661209106445</v>
       </c>
     </row>
     <row r="4">
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9112033843994141</v>
+        <v>0.8815181255340576</v>
       </c>
     </row>
     <row r="5">
@@ -521,10 +521,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6715229749679565</v>
+        <v>0.4906995892524719</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.198024719953537</v>
+        <v>0.03579447790980339</v>
       </c>
     </row>
     <row r="7">
@@ -560,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9465768337249756</v>
+        <v>0.8550922870635986</v>
       </c>
     </row>
     <row r="8">
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.684072732925415</v>
+        <v>0.6009546518325806</v>
       </c>
     </row>
     <row r="9">
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.473397970199585</v>
+        <v>0.2650291323661804</v>
       </c>
     </row>
     <row r="10">
@@ -614,7 +614,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5302512645721436</v>
+        <v>0.6092824935913086</v>
       </c>
     </row>
     <row r="11">
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2255795747041702</v>
+        <v>0.2607499063014984</v>
       </c>
     </row>
     <row r="12">
@@ -650,7 +650,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3095614314079285</v>
+        <v>0.3480855822563171</v>
       </c>
     </row>
     <row r="13">
@@ -668,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8774191737174988</v>
+        <v>0.9318639039993286</v>
       </c>
     </row>
     <row r="14">
@@ -686,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8964925408363342</v>
+        <v>0.8949315547943115</v>
       </c>
     </row>
     <row r="15">
@@ -701,10 +701,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.554570198059082</v>
+        <v>0.4818087816238403</v>
       </c>
     </row>
     <row r="16">
@@ -719,10 +719,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.7132629752159119</v>
+        <v>0.2817938923835754</v>
       </c>
     </row>
     <row r="17">
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8830661177635193</v>
+        <v>0.6917387843132019</v>
       </c>
     </row>
     <row r="18">
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8064461946487427</v>
+        <v>0.6596561670303345</v>
       </c>
     </row>
     <row r="19">
@@ -773,10 +773,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5176265239715576</v>
+        <v>0.4472375214099884</v>
       </c>
     </row>
     <row r="20">
@@ -791,10 +791,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5133489966392517</v>
+        <v>0.3857227563858032</v>
       </c>
     </row>
     <row r="21">
@@ -812,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2200243026018143</v>
+        <v>0.3868101835250854</v>
       </c>
     </row>
     <row r="22">
@@ -830,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5478384494781494</v>
+        <v>0.6083816289901733</v>
       </c>
     </row>
     <row r="23">
@@ -848,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7173118591308594</v>
+        <v>0.8168272376060486</v>
       </c>
     </row>
     <row r="24">
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4508552849292755</v>
+        <v>0.4704257249832153</v>
       </c>
     </row>
     <row r="25">
@@ -884,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>0.8262330889701843</v>
+        <v>0.6048879623413086</v>
       </c>
     </row>
     <row r="26">
@@ -902,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>0.934478759765625</v>
+        <v>0.8973966836929321</v>
       </c>
     </row>
     <row r="27">
@@ -920,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4743472039699554</v>
+        <v>0.09893088042736053</v>
       </c>
     </row>
     <row r="28">
@@ -938,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>0.6623991727828979</v>
+        <v>0.7424843311309814</v>
       </c>
     </row>
     <row r="29">
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2277339100837708</v>
+        <v>0.2871742844581604</v>
       </c>
     </row>
     <row r="30">
@@ -974,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>0.6854764223098755</v>
+        <v>0.7195528745651245</v>
       </c>
     </row>
     <row r="31">
@@ -992,7 +992,7 @@
         <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5086690783500671</v>
+        <v>0.6281295418739319</v>
       </c>
     </row>
     <row r="32">
@@ -1007,10 +1007,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0.6448900699615479</v>
+        <v>0.4695977568626404</v>
       </c>
     </row>
     <row r="33">
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>0.7915782928466797</v>
+        <v>0.7509008049964905</v>
       </c>
     </row>
     <row r="34">
@@ -1046,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9039463996887207</v>
+        <v>0.8773109316825867</v>
       </c>
     </row>
     <row r="35">
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>0.6719736456871033</v>
+        <v>0.6579916477203369</v>
       </c>
     </row>
     <row r="36">
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.2903981804847717</v>
+        <v>0.1931407898664474</v>
       </c>
     </row>
     <row r="37">
@@ -1100,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>0.682597279548645</v>
+        <v>0.6744139194488525</v>
       </c>
     </row>
     <row r="38">
@@ -1118,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>0.6052093505859375</v>
+        <v>0.6589869260787964</v>
       </c>
     </row>
     <row r="39">
@@ -1136,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>0.8350102305412292</v>
+        <v>0.9035844206809998</v>
       </c>
     </row>
     <row r="40">
@@ -1154,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8173097372055054</v>
+        <v>0.8995659351348877</v>
       </c>
     </row>
     <row r="41">
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>0.9269909262657166</v>
+        <v>0.9240585565567017</v>
       </c>
     </row>
     <row r="42">
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>0.4373602569103241</v>
+        <v>0.472154289484024</v>
       </c>
     </row>
     <row r="43">
@@ -1208,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>0.5490264892578125</v>
+        <v>0.6990923881530762</v>
       </c>
     </row>
     <row r="44">
@@ -1226,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>0.5116506814956665</v>
+        <v>0.50604248046875</v>
       </c>
     </row>
     <row r="45">
@@ -1244,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.3559271395206451</v>
+        <v>0.3106720745563507</v>
       </c>
     </row>
     <row r="46">
@@ -1262,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="D46" t="n">
-        <v>0.8489736318588257</v>
+        <v>0.7669169306755066</v>
       </c>
     </row>
     <row r="47">
@@ -1280,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>0.6824671030044556</v>
+        <v>0.7663993835449219</v>
       </c>
     </row>
     <row r="48">
@@ -1295,10 +1295,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.6174136996269226</v>
+        <v>0.4958132207393646</v>
       </c>
     </row>
     <row r="49">
@@ -1316,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.4476843476295471</v>
+        <v>0.4251040816307068</v>
       </c>
     </row>
     <row r="50">
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>0.4695099294185638</v>
+        <v>0.3030686676502228</v>
       </c>
     </row>
     <row r="51">
@@ -1349,10 +1349,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>0.5353732705116272</v>
+        <v>0.4973229169845581</v>
       </c>
     </row>
     <row r="52">
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>0.1604891270399094</v>
+        <v>0.04164242371916771</v>
       </c>
     </row>
     <row r="53">
@@ -1388,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>0.4576481878757477</v>
+        <v>0.4022634327411652</v>
       </c>
     </row>
     <row r="54">
@@ -1406,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="D54" t="n">
-        <v>0.8174224495887756</v>
+        <v>0.7426232099533081</v>
       </c>
     </row>
     <row r="55">
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.3048042058944702</v>
+        <v>0.301032692193985</v>
       </c>
     </row>
     <row r="56">
@@ -1442,7 +1442,7 @@
         <v>1</v>
       </c>
       <c r="D56" t="n">
-        <v>0.5008374452590942</v>
+        <v>0.5794994831085205</v>
       </c>
     </row>
     <row r="57">
@@ -1460,7 +1460,7 @@
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>0.3472401797771454</v>
+        <v>0.3193793296813965</v>
       </c>
     </row>
     <row r="58">
@@ -1475,10 +1475,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>0.7781393527984619</v>
+        <v>0.4921939074993134</v>
       </c>
     </row>
     <row r="59">
@@ -1493,10 +1493,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0.5788542032241821</v>
+        <v>0.4344651699066162</v>
       </c>
     </row>
     <row r="60">
@@ -1514,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>0.8915619850158691</v>
+        <v>0.8449845910072327</v>
       </c>
     </row>
     <row r="61">
@@ -1532,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>0.7705929279327393</v>
+        <v>0.660047173500061</v>
       </c>
     </row>
     <row r="62">
@@ -1550,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="D62" t="n">
-        <v>0.6794452667236328</v>
+        <v>0.7874123454093933</v>
       </c>
     </row>
     <row r="63">
@@ -1568,7 +1568,7 @@
         <v>1</v>
       </c>
       <c r="D63" t="n">
-        <v>0.7870506048202515</v>
+        <v>0.601777970790863</v>
       </c>
     </row>
     <row r="64">
@@ -1586,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>0.3778361976146698</v>
+        <v>0.2680604457855225</v>
       </c>
     </row>
     <row r="65">
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2814287841320038</v>
+        <v>0.1983697563409805</v>
       </c>
     </row>
     <row r="66">
@@ -1622,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="D66" t="n">
-        <v>0.8405328989028931</v>
+        <v>0.6706690788269043</v>
       </c>
     </row>
     <row r="67">
@@ -1640,7 +1640,7 @@
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>0.4315721094608307</v>
+        <v>0.2993455231189728</v>
       </c>
     </row>
     <row r="68">
@@ -1658,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="D68" t="n">
-        <v>0.5881571769714355</v>
+        <v>0.6111308932304382</v>
       </c>
     </row>
     <row r="69">
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
       <c r="D69" t="n">
-        <v>0.6431185007095337</v>
+        <v>0.6785590052604675</v>
       </c>
     </row>
     <row r="70">
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2377204895019531</v>
+        <v>0.2101347744464874</v>
       </c>
     </row>
     <row r="71">
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>0.4428095817565918</v>
+        <v>0.3166807889938354</v>
       </c>
     </row>
     <row r="72">
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>0.4955498576164246</v>
+        <v>0.1608679294586182</v>
       </c>
     </row>
     <row r="73">
@@ -1748,7 +1748,7 @@
         <v>1</v>
       </c>
       <c r="D73" t="n">
-        <v>0.8746345043182373</v>
+        <v>0.7539152503013611</v>
       </c>
     </row>
     <row r="74">
@@ -1766,7 +1766,7 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>0.450461357831955</v>
+        <v>0.4324472844600677</v>
       </c>
     </row>
     <row r="75">
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>0.2036319226026535</v>
+        <v>0.1621224731206894</v>
       </c>
     </row>
     <row r="76">
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>0.2354903817176819</v>
+        <v>0.4747454226016998</v>
       </c>
     </row>
     <row r="77">
@@ -1820,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="D77" t="n">
-        <v>0.6538888216018677</v>
+        <v>0.5858806371688843</v>
       </c>
     </row>
     <row r="78">
@@ -1838,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="D78" t="n">
-        <v>0.6643117070198059</v>
+        <v>0.6373843550682068</v>
       </c>
     </row>
     <row r="79">
@@ -1856,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>0.2507842183113098</v>
+        <v>0.3585901260375977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved project for data scraping
</commit_message>
<xml_diff>
--- a/predictions/classical_predictions.xlsx
+++ b/predictions/classical_predictions.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -463,392 +463,392 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Green Bay Packers</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4480947554111481</v>
+        <v>0.6487739682197571</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Minnesota Vikings</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kansas City Chiefs</t>
+          <t>Washington Commanders</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3647661209106445</v>
+        <v>0.4194351136684418</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Baltimore Ravens</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals</t>
+          <t>Miami Dolphins</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8815181255340576</v>
+        <v>0.2461310923099518</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Chicago Bears</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4906995892524719</v>
+        <v>0.2874460518360138</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tennessee Titans</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.03579447790980339</v>
+        <v>0.5571020841598511</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>New Orleans Saints</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8550922870635986</v>
+        <v>0.7998444437980652</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Miami Dolphins</t>
+          <t>Jacksonville Jaguars</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>New Orleans Saints</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6009546518325806</v>
+        <v>0.5188615918159485</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>Tennessee Titans</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2650291323661804</v>
+        <v>0.6463430523872375</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>Cincinnati Bengals</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6092824935913086</v>
+        <v>0.8727564215660095</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Carolina Panthers</t>
+          <t>Las Vegas Raiders</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Denver Broncos</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2607499063014984</v>
+        <v>0.1347152292728424</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>Green Bay Packers</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>San Francisco 49ers</t>
+          <t>Chicago Bears</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3480855822563171</v>
+        <v>0.6946927309036255</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Arizona Cardinals</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9318639039993286</v>
+        <v>0.2467021644115448</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers</t>
+          <t>Kansas City Chiefs</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8949315547943115</v>
+        <v>0.7214451432228088</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Los Angeles Chargers</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4818087816238403</v>
+        <v>0.6869970560073853</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2817938923835754</v>
+        <v>0.6564435362815857</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>New England Patriots</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>New York Giants</t>
+          <t>Arizona Cardinals</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6917387843132019</v>
+        <v>0.7107254862785339</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Detroit Lions</t>
+          <t>Chicago Bears</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="C18" t="n">
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6596561670303345</v>
+        <v>0.9390183687210083</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>Kansas City Chiefs</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>Los Angeles Chargers</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4472375214099884</v>
+        <v>0.5399633646011353</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>Cincinnati Bengals</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Miami Dolphins</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3857227563858032</v>
+        <v>0.3771255910396576</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>New England Patriots</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3868101835250854</v>
+        <v>0.5452147722244263</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Baltimore Ravens</t>
+          <t>New York Giants</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Washington Commanders</t>
         </is>
       </c>
       <c r="C22" t="n">
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6083816289901733</v>
+        <v>0.6943840980529785</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>New Orleans Saints</t>
+          <t>Las Vegas Raiders</t>
         </is>
       </c>
       <c r="C23" t="n">
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8168272376060486</v>
+        <v>0.7975617051124573</v>
       </c>
     </row>
     <row r="24">
@@ -859,20 +859,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4704257249832153</v>
+        <v>0.9401481747627258</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>San Francisco 49ers</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -884,175 +884,175 @@
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>0.6048879623413086</v>
+        <v>0.9705215692520142</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="C26" t="n">
         <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>0.8973966836929321</v>
+        <v>0.6438053846359253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Detroit Lions</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>0.09893088042736053</v>
+        <v>0.8435688614845276</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Denver Broncos</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>Green Bay Packers</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Chicago Bears</t>
-        </is>
-      </c>
       <c r="C28" t="n">
         <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7424843311309814</v>
+        <v>0.5077956914901733</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>New Orleans Saints</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Carolina Panthers</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2871742844581604</v>
+        <v>0.5068655014038086</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Kansas City Chiefs</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>Minnesota Vikings</t>
         </is>
       </c>
       <c r="C30" t="n">
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7195528745651245</v>
+        <v>0.8942446708679199</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Miami Dolphins</t>
         </is>
       </c>
       <c r="C31" t="n">
         <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>0.6281295418739319</v>
+        <v>0.6404906511306763</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>0.4695977568626404</v>
+        <v>0.6416428089141846</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>Chicago Bears</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>Green Bay Packers</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0.7509008049964905</v>
+        <v>0.4903823435306549</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Chicago Bears</t>
+          <t>Washington Commanders</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>0.8773109316825867</v>
+        <v>0.3771119713783264</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Kansas City Chiefs</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1064,43 +1064,43 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>0.6579916477203369</v>
+        <v>0.6265697479248047</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals</t>
+          <t>Tennessee Titans</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Baltimore Ravens</t>
+          <t>Kansas City Chiefs</t>
         </is>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1931407898664474</v>
+        <v>0.1345992833375931</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>New England Patriots</t>
+          <t>New Orleans Saints</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="C37" t="n">
         <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>0.6744139194488525</v>
+        <v>0.799930214881897</v>
       </c>
     </row>
     <row r="38">
@@ -1111,590 +1111,590 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>Minnesota Vikings</t>
         </is>
       </c>
       <c r="C38" t="n">
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>0.6589869260787964</v>
+        <v>0.7714910507202148</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Carolina Panthers</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>0.9035844206809998</v>
+        <v>0.4489836096763611</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8995659351348877</v>
+        <v>0.2727896869182587</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>San Francisco 49ers</t>
+          <t>Miami Dolphins</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Tennessee Titans</t>
+          <t>Cincinnati Bengals</t>
         </is>
       </c>
       <c r="C41" t="n">
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>0.9240585565567017</v>
+        <v>0.6959856748580933</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Denver Broncos</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>Jacksonville Jaguars</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>0.472154289484024</v>
+        <v>0.5401009917259216</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Arizona Cardinals</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Detroit Lions</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="C43" t="n">
         <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>0.6990923881530762</v>
+        <v>0.5106133818626404</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Green Bay Packers</t>
+          <t>Las Vegas Raiders</t>
         </is>
       </c>
       <c r="C44" t="n">
         <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>0.50604248046875</v>
+        <v>0.8056070804595947</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>New Orleans Saints</t>
+          <t>Detroit Lions</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Carolina Panthers</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>0.3106720745563507</v>
+        <v>0.6076276302337646</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>New England Patriots</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>0.7669169306755066</v>
+        <v>0.2944760620594025</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Miami Dolphins</t>
+          <t>San Francisco 49ers</t>
         </is>
       </c>
       <c r="C47" t="n">
         <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>0.7663993835449219</v>
+        <v>0.5699698925018311</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Washington Commanders</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.4958132207393646</v>
+        <v>0.2946124076843262</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Chicago Bears</t>
+          <t>Minnesota Vikings</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Green Bay Packers</t>
+          <t>Detroit Lions</t>
         </is>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.4251040816307068</v>
+        <v>0.1952850371599197</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>Kansas City Chiefs</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Denver Broncos</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" t="n">
-        <v>0.3030686676502228</v>
+        <v>0.5469412207603455</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Las Vegas Raiders</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers</t>
+          <t>New York Giants</t>
         </is>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>0.4973229169845581</v>
+        <v>0.3048562407493591</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Tennessee Titans</t>
+          <t>Los Angeles Chargers</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Kansas City Chiefs</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>0.04164242371916771</v>
+        <v>0.6447190642356873</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>New Orleans Saints</t>
+          <t>Green Bay Packers</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>0.4022634327411652</v>
+        <v>0.7965420484542847</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>New York Giants</t>
+          <t>Carolina Panthers</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.7426232099533081</v>
+        <v>0.3136469125747681</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Baltimore Ravens</t>
+          <t>Cincinnati Bengals</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>New England Patriots</t>
+          <t>Arizona Cardinals</t>
         </is>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.301032692193985</v>
+        <v>0.3540443480014801</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Carolina Panthers</t>
+          <t>Tennessee Titans</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers</t>
+          <t>New Orleans Saints</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>0.5794994831085205</v>
+        <v>0.3248816728591919</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>Jacksonville Jaguars</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>0.3193793296813965</v>
+        <v>0.692084789276123</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Miami Dolphins</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="C58" t="n">
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>0.4921939074993134</v>
+        <v>0.4114691913127899</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>New England Patriots</t>
         </is>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0.4344651699066162</v>
+        <v>0.1081416308879852</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="C60" t="n">
         <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>0.8449845910072327</v>
+        <v>0.5753545761108398</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Detroit Lions</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="C61" t="n">
         <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>0.660047173500061</v>
+        <v>0.6864956021308899</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Miami Dolphins</t>
+          <t>San Francisco 49ers</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals</t>
+          <t>Chicago Bears</t>
         </is>
       </c>
       <c r="C62" t="n">
         <v>1</v>
       </c>
       <c r="D62" t="n">
-        <v>0.7874123454093933</v>
+        <v>0.5425477623939514</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>San Francisco 49ers</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>0.601777970790863</v>
+        <v>0.3399148285388947</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>Las Vegas Raiders</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Kansas City Chiefs</t>
         </is>
       </c>
       <c r="C64" t="n">
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2680604457855225</v>
+        <v>0.1444612890481949</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Detroit Lions</t>
+          <t>Arizona Cardinals</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" t="n">
-        <v>0.1983697563409805</v>
+        <v>0.9419038891792297</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Kansas City Chiefs</t>
+          <t>San Francisco 49ers</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>0.6706690788269043</v>
+        <v>0.3225615918636322</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Denver Broncos</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>New York Giants</t>
+          <t>Los Angeles Chargers</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2993455231189728</v>
+        <v>0.6526976823806763</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="C68" t="n">
         <v>1</v>
       </c>
       <c r="D68" t="n">
-        <v>0.6111308932304382</v>
+        <v>0.5864806175231934</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>Minnesota Vikings</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
           <t>Green Bay Packers</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Baltimore Ravens</t>
-        </is>
-      </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>0.6785590052604675</v>
+        <v>0.1747644543647766</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Carolina Panthers</t>
+          <t>Chicago Bears</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Detroit Lions</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2101347744464874</v>
+        <v>0.5633623600006104</v>
       </c>
     </row>
     <row r="71">
@@ -1705,20 +1705,20 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71" t="n">
-        <v>0.3166807889938354</v>
+        <v>0.8890040516853333</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Tennessee Titans</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1727,136 +1727,136 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72" t="n">
-        <v>0.1608679294586182</v>
+        <v>0.6136543750762939</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="C73" t="n">
         <v>1</v>
       </c>
       <c r="D73" t="n">
-        <v>0.7539152503013611</v>
+        <v>0.9532912969589233</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
+          <t>New England Patriots</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
           <t>Miami Dolphins</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Tampa Bay Buccaneers</t>
-        </is>
-      </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" t="n">
-        <v>0.4324472844600677</v>
+        <v>0.7925955057144165</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>New York Giants</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>New England Patriots</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="C75" t="n">
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>0.1621224731206894</v>
+        <v>0.4446119070053101</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Washington Commanders</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76" t="n">
-        <v>0.4747454226016998</v>
+        <v>0.6290091276168823</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="C77" t="n">
         <v>1</v>
       </c>
       <c r="D77" t="n">
-        <v>0.5858806371688843</v>
+        <v>0.5123748183250427</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>San Francisco 49ers</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Chicago Bears</t>
+          <t>Carolina Panthers</t>
         </is>
       </c>
       <c r="C78" t="n">
         <v>1</v>
       </c>
       <c r="D78" t="n">
-        <v>0.6373843550682068</v>
+        <v>0.5896153450012207</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>Jacksonville Jaguars</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Tennessee Titans</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79" t="n">
-        <v>0.3585901260375977</v>
+        <v>0.9365166425704956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>